<commit_message>
importamos e exportamos, só falta o histórico
</commit_message>
<xml_diff>
--- a/integrador/api_smart/excel/contador.xlsx
+++ b/integrador/api_smart/excel/contador.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\2DSTB-12\Disciplinas\PWBE\Integrador\Dados Integrador\Dados Integrador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43705577808\Desktop\PWBE\integrador\api_smart\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46B5313-96AE-448E-9C78-143AC1425F69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAC0955-4AF0-403F-A018-5D5DB7D15960}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="15">
   <si>
     <t>sensor</t>
   </si>
@@ -58,17 +58,20 @@
     <t>uni</t>
   </si>
   <si>
-    <t>true</t>
+    <t>ativo</t>
   </si>
   <si>
-    <t>false</t>
+    <t>inativo</t>
+  </si>
+  <si>
+    <t>00:1B:44:11:3A:BP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +81,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,11 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:H205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="H197" sqref="H197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4318,7 +4330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>6</v>
       </c>
@@ -4338,7 +4350,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>6</v>
       </c>
@@ -4358,7 +4370,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>6</v>
       </c>
@@ -4378,7 +4390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>6</v>
       </c>
@@ -4398,7 +4410,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>6</v>
       </c>
@@ -4418,7 +4430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>6</v>
       </c>
@@ -4438,7 +4450,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>6</v>
       </c>
@@ -4458,7 +4470,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>6</v>
       </c>
@@ -4477,8 +4489,9 @@
       <c r="F200" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H200" s="2"/>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>6</v>
       </c>
@@ -4498,7 +4511,31 @@
         <v>12</v>
       </c>
     </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>6</v>
+      </c>
+      <c r="B202" t="s">
+        <v>14</v>
+      </c>
+      <c r="C202" t="s">
+        <v>11</v>
+      </c>
+      <c r="D202">
+        <v>-86.987639999999999</v>
+      </c>
+      <c r="E202">
+        <v>-25.874500000000001</v>
+      </c>
+      <c r="F202" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H205" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>